<commit_message>
script changes done related to future rates
</commit_message>
<xml_diff>
--- a/Inputs/Ison_Secure/info.xlsx
+++ b/Inputs/Ison_Secure/info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">provider</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">insurerName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">futureRates</t>
   </si>
   <si>
     <t xml:space="preserve">ison</t>
@@ -77,11 +80,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -102,6 +106,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -159,7 +168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -172,15 +181,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -264,17 +281,17 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.65"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -302,42 +319,47 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="K1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="7" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>